<commit_message>
added login home page
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Github\online-appointment-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9551CB56-ECCE-4E88-816C-5F3E8D0A0F79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CB7A3D-9671-41DE-BCD8-A1B165932804}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8025" yWindow="690" windowWidth="19950" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -1416,13 +1416,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F7" s="7">
         <v>1</v>
       </c>
       <c r="G7" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1456,13 +1456,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F9" s="7">
         <v>1</v>
       </c>
       <c r="G9" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: added registration form page
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Github\online-appointment-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CB7A3D-9671-41DE-BCD8-A1B165932804}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19C3756-77D4-4D5E-A4BF-42A76163276B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8025" yWindow="690" windowWidth="19950" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -174,13 +174,13 @@
     <t>Create select application pages html</t>
   </si>
   <si>
-    <t>Create interface for reviewer</t>
-  </si>
-  <si>
     <t>CSS</t>
   </si>
   <si>
     <t>Application App</t>
+  </si>
+  <si>
+    <t>Create interface and backend for reviewer</t>
   </si>
 </sst>
 </file>
@@ -1007,7 +1007,7 @@
   <dimension ref="B1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1021,7 +1021,7 @@
   <sheetData>
     <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -1436,13 +1436,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F8" s="7">
         <v>1</v>
       </c>
       <c r="G8" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1513,7 +1513,7 @@
         <v>7</v>
       </c>
       <c r="D12" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="7">
         <v>1</v>
@@ -1527,13 +1527,13 @@
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C13" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D13" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="7">
         <v>1</v>
@@ -1547,10 +1547,10 @@
     </row>
     <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="7">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D14" s="7">
         <v>2</v>

</xml_diff>